<commit_message>
Implementat el generador i avaluador d'Oliva (1992) que diferencia els valors dels batecs accentuals (0-3).
</commit_message>
<xml_diff>
--- a/generated/dols2006.xlsx
+++ b/generated/dols2006.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RM1</t>
+          <t>RC2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RM2</t>
+          <t>RC3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -461,19 +461,19 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>RM1 posicions</t>
+          <t>RC2 posicions</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>RM2 posicions</t>
+          <t>RC3 posicions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TAATATAAAT</t>
+          <t>ATATATATAT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -482,29 +482,21 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2, 8</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ATAAATATAT</t>
+          <t>AAATATATAT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -513,25 +505,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AAAAATAAAT</t>
+          <t>ATAAATATAT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -540,20 +532,20 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>4, 8</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,20 +559,20 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -594,29 +586,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TAAAATAAAT</t>
+          <t>ATAAATAAAT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -625,29 +613,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>2</v>
       </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>4, 8</t>
-        </is>
-      </c>
+          <t>3, 7</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AAATATATAT</t>
+          <t>TAATATAAAT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -656,25 +640,29 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AAATATAAAT</t>
+          <t>TAAAATATAT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -683,18 +671,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2, 8</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -710,25 +702,25 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1, 3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ATATATATAT</t>
+          <t>AAATATAAAT</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -737,21 +729,25 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1, 7</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ATAAATAAAT</t>
+          <t>AAAAATAAAT</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -760,25 +756,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>4, 8</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1, 3, 7</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TAAAATATAT</t>
+          <t>TAAAATAAAT</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -787,22 +783,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>3, 7</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Afegit mòdul de comparació.
</commit_message>
<xml_diff>
--- a/generated/dols2006.xlsx
+++ b/generated/dols2006.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,55 +434,55 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Exemple</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>RC2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>RC3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Complexitat</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>RC2 posicions</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>RC3 posicions</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>ATATATATAT</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -490,313 +490,349 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATATATAAAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AAATATATAT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ATAAATATAT</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ATATATAAAT</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TAATATATAT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AAAAATATAT</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1, 3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TAATATAAAT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TAATATATAT</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>AAATATATAT</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ATAAATAAAT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>3, 7</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AAATATAAAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1, 7</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TAAAATATAT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TAAAATATAT</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>AAAAATATAT</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>1, 3</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>AAATATAAAT</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1, 7</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ATAAATAAAT</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" t="inlineStr">
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AAAAATAAAT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1, 3, 7</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TAAAATAAAT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>WSWSWSWSWS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>3, 7</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>TAATATAAAT</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>AAAAATAAAT</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>1, 3, 7</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>TAAAATAAAT</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>WSWSWSWSWS</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>3, 7</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>1</t>
         </is>

</xml_diff>

<commit_message>
Desenvolupant mòdul de comparació.
</commit_message>
<xml_diff>
--- a/generated/dols2006.xlsx
+++ b/generated/dols2006.xlsx
@@ -502,7 +502,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ATATATAAAT</t>
+          <t>TAATATATAT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -511,20 +511,20 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -562,7 +562,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ATAAATATAT</t>
+          <t>ATATATAAAT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -592,7 +592,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TAATATATAT</t>
+          <t>ATAAATATAT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -601,20 +601,20 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -622,7 +622,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AAAAATATAT</t>
+          <t>TAATATAAAT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -631,20 +631,24 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1, 3</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -652,7 +656,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TAATATAAAT</t>
+          <t>ATAAATAAAT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -661,24 +665,20 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>2</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>3, 7</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ATAAATAAAT</t>
+          <t>TAAAATATAT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -695,20 +695,24 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3, 7</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -716,7 +720,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AAATATAAAT</t>
+          <t>AAAAATATAT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -735,7 +739,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1, 7</t>
+          <t>1, 3</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -746,7 +750,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TAAAATATAT</t>
+          <t>AAATATAAAT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -755,24 +759,20 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>2</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>1, 7</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -780,7 +780,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AAAAATAAAT</t>
+          <t>TAAAATAAAT</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -789,20 +789,24 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>3</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1, 3, 7</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
+          <t>3, 7</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -810,7 +814,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TAAAATAAAT</t>
+          <t>AAAAATAAAT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -819,24 +823,20 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>3</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3, 7</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>1, 3, 7</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>